<commit_message>
jones mapbox scatter plot map
-using mapbox for jones maps, in the middle of editing code for style
- but code works, got px.scatter working but can't customize.
-added a lot notes and links
</commit_message>
<xml_diff>
--- a/SheilaJones_Miran_review.xlsx
+++ b/SheilaJones_Miran_review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curryt/Documents/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curryt/Documents/GitHub/AWHI-projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEE06D5A-AEDF-FA4F-B2B5-4B29C4186CF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49902CFE-CA0B-4D43-B7EA-7B37CCD86A72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="4720" windowWidth="28800" windowHeight="17540" xr2:uid="{DFCE0D8B-6B2C-E045-BFA6-1B2BFEAAC0E1}"/>
+    <workbookView xWindow="67980" yWindow="3160" windowWidth="28800" windowHeight="17540" xr2:uid="{DFCE0D8B-6B2C-E045-BFA6-1B2BFEAAC0E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>